<commit_message>
households compositions single adult
</commit_message>
<xml_diff>
--- a/data_output/eng_plot_input.xlsx
+++ b/data_output/eng_plot_input.xlsx
@@ -293,34 +293,34 @@
     <t>88</t>
   </si>
   <si>
-    <t>Less 200</t>
-  </si>
-  <si>
-    <t>200 to 400</t>
-  </si>
-  <si>
-    <t>400 to 600</t>
-  </si>
-  <si>
-    <t>600 to 800</t>
-  </si>
-  <si>
-    <t>800 to 1000</t>
-  </si>
-  <si>
-    <t>1000 to 1200</t>
-  </si>
-  <si>
-    <t>1200 to 1400</t>
-  </si>
-  <si>
-    <t>1400 to 1600</t>
-  </si>
-  <si>
-    <t>1600 to 1800</t>
-  </si>
-  <si>
-    <t>1800 to 2000</t>
+    <t>Less than 200</t>
+  </si>
+  <si>
+    <t>200 and less than  400</t>
+  </si>
+  <si>
+    <t>400 and less than 600</t>
+  </si>
+  <si>
+    <t>600 and less than 800</t>
+  </si>
+  <si>
+    <t>800 and less than 1000</t>
+  </si>
+  <si>
+    <t>1000 and less than 1200</t>
+  </si>
+  <si>
+    <t>1200 and less than 1400</t>
+  </si>
+  <si>
+    <t>1400 and less than 1600</t>
+  </si>
+  <si>
+    <t>1600 and less than 1800</t>
+  </si>
+  <si>
+    <t>1800 and less than 2000</t>
   </si>
   <si>
     <t>Above 2000</t>
@@ -409,7 +409,7 @@
         <v>2459.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.08540056933712892</v>
+        <v>8.540056933712892</v>
       </c>
     </row>
     <row r="3">
@@ -429,7 +429,7 @@
         <v>2459.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.35258235054900366</v>
+        <v>35.25823505490037</v>
       </c>
     </row>
     <row r="4">
@@ -449,7 +449,7 @@
         <v>2459.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2635217568117121</v>
+        <v>26.352175681171207</v>
       </c>
     </row>
     <row r="5">
@@ -469,7 +469,7 @@
         <v>2459.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.13867425782838552</v>
+        <v>13.867425782838552</v>
       </c>
     </row>
     <row r="6">
@@ -489,7 +489,7 @@
         <v>2459.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.07523383489223262</v>
+        <v>7.523383489223262</v>
       </c>
     </row>
     <row r="7">
@@ -509,7 +509,7 @@
         <v>2459.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.040666937779585195</v>
+        <v>4.06669377795852</v>
       </c>
     </row>
     <row r="8">
@@ -529,7 +529,7 @@
         <v>2459.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.017486783245221633</v>
+        <v>1.7486783245221633</v>
       </c>
     </row>
     <row r="9">
@@ -549,7 +549,7 @@
         <v>2459.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.011793411956079707</v>
+        <v>1.1793411956079707</v>
       </c>
     </row>
     <row r="10">
@@ -569,7 +569,7 @@
         <v>2459.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0061000406669377795</v>
+        <v>0.6100040666937779</v>
       </c>
     </row>
     <row r="11">
@@ -589,7 +589,7 @@
         <v>2459.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0028466856445709637</v>
+        <v>0.2846685644570964</v>
       </c>
     </row>
     <row r="12">
@@ -609,7 +609,7 @@
         <v>2459.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0056933712891419274</v>
+        <v>0.5693371289141927</v>
       </c>
     </row>
     <row r="13">
@@ -629,7 +629,7 @@
         <v>2211.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.07055630936227951</v>
+        <v>7.055630936227951</v>
       </c>
     </row>
     <row r="14">
@@ -649,7 +649,7 @@
         <v>2211.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.23473541383989144</v>
+        <v>23.473541383989144</v>
       </c>
     </row>
     <row r="15">
@@ -669,7 +669,7 @@
         <v>2211.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.22749886928991406</v>
+        <v>22.749886928991405</v>
       </c>
     </row>
     <row r="16">
@@ -689,7 +689,7 @@
         <v>2211.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1560379918588874</v>
+        <v>15.60379918588874</v>
       </c>
     </row>
     <row r="17">
@@ -709,7 +709,7 @@
         <v>2211.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.11578471279963817</v>
+        <v>11.578471279963818</v>
       </c>
     </row>
     <row r="18">
@@ -729,7 +729,7 @@
         <v>2211.0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0814111261872456</v>
+        <v>8.14111261872456</v>
       </c>
     </row>
     <row r="19">
@@ -749,7 +749,7 @@
         <v>2211.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.04613297150610583</v>
+        <v>4.613297150610583</v>
       </c>
     </row>
     <row r="20">
@@ -769,7 +769,7 @@
         <v>2211.0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.031207598371777476</v>
+        <v>3.1207598371777476</v>
       </c>
     </row>
     <row r="21">
@@ -789,7 +789,7 @@
         <v>2211.0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.012211668928086838</v>
+        <v>1.2211668928086838</v>
       </c>
     </row>
     <row r="22">
@@ -809,7 +809,7 @@
         <v>2211.0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.008593396653098146</v>
+        <v>0.8593396653098146</v>
       </c>
     </row>
     <row r="23">
@@ -829,7 +829,7 @@
         <v>2211.0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.015829941203075532</v>
+        <v>1.5829941203075533</v>
       </c>
     </row>
     <row r="24">
@@ -849,7 +849,7 @@
         <v>2686.0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.05956813104988831</v>
+        <v>5.956813104988831</v>
       </c>
     </row>
     <row r="25">
@@ -869,7 +869,7 @@
         <v>2686.0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.17051377513030527</v>
+        <v>17.051377513030527</v>
       </c>
     </row>
     <row r="26">
@@ -889,7 +889,7 @@
         <v>2686.0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.19806403574087864</v>
+        <v>19.806403574087863</v>
       </c>
     </row>
     <row r="27">
@@ -909,7 +909,7 @@
         <v>2686.0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.14556962025316456</v>
+        <v>14.556962025316455</v>
       </c>
     </row>
     <row r="28">
@@ -929,7 +929,7 @@
         <v>2686.0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.11913626209977662</v>
+        <v>11.913626209977663</v>
       </c>
     </row>
     <row r="29">
@@ -949,7 +949,7 @@
         <v>2686.0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.10014892032762472</v>
+        <v>10.014892032762472</v>
       </c>
     </row>
     <row r="30">
@@ -969,7 +969,7 @@
         <v>2686.0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06142963514519732</v>
+        <v>6.1429635145197325</v>
       </c>
     </row>
     <row r="31">
@@ -989,7 +989,7 @@
         <v>2686.0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.045420699925539834</v>
+        <v>4.542069992553984</v>
       </c>
     </row>
     <row r="32">
@@ -1009,7 +1009,7 @@
         <v>2686.0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.033879374534623974</v>
+        <v>3.3879374534623974</v>
       </c>
     </row>
     <row r="33">
@@ -1029,7 +1029,7 @@
         <v>2686.0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.020104244229337303</v>
+        <v>2.0104244229337302</v>
       </c>
     </row>
     <row r="34">
@@ -1049,7 +1049,7 @@
         <v>2686.0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.04616530156366344</v>
+        <v>4.616530156366344</v>
       </c>
     </row>
     <row r="35">
@@ -1069,7 +1069,7 @@
         <v>2036.0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.05157170923379175</v>
+        <v>5.157170923379175</v>
       </c>
     </row>
     <row r="36">
@@ -1089,7 +1089,7 @@
         <v>2036.0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.12622789783889982</v>
+        <v>12.622789783889981</v>
       </c>
     </row>
     <row r="37">
@@ -1109,7 +1109,7 @@
         <v>2036.0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.16306483300589392</v>
+        <v>16.30648330058939</v>
       </c>
     </row>
     <row r="38">
@@ -1129,7 +1129,7 @@
         <v>2036.0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.15029469548133595</v>
+        <v>15.029469548133594</v>
       </c>
     </row>
     <row r="39">
@@ -1149,7 +1149,7 @@
         <v>2036.0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.11886051080550099</v>
+        <v>11.886051080550098</v>
       </c>
     </row>
     <row r="40">
@@ -1169,7 +1169,7 @@
         <v>2036.0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.09135559921414538</v>
+        <v>9.135559921414538</v>
       </c>
     </row>
     <row r="41">
@@ -1189,7 +1189,7 @@
         <v>2036.0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.07809430255402751</v>
+        <v>7.809430255402751</v>
       </c>
     </row>
     <row r="42">
@@ -1209,7 +1209,7 @@
         <v>2036.0</v>
       </c>
       <c r="F42" t="n">
-        <v>0.05992141453831041</v>
+        <v>5.992141453831041</v>
       </c>
     </row>
     <row r="43">
@@ -1229,7 +1229,7 @@
         <v>2036.0</v>
       </c>
       <c r="F43" t="n">
-        <v>0.04174852652259332</v>
+        <v>4.174852652259331</v>
       </c>
     </row>
     <row r="44">
@@ -1249,7 +1249,7 @@
         <v>2036.0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.029469548133595286</v>
+        <v>2.9469548133595285</v>
       </c>
     </row>
     <row r="45">
@@ -1269,7 +1269,7 @@
         <v>2036.0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.0893909626719057</v>
+        <v>8.93909626719057</v>
       </c>
     </row>
     <row r="46">
@@ -1289,7 +1289,7 @@
         <v>1290.0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.04108527131782946</v>
+        <v>4.108527131782946</v>
       </c>
     </row>
     <row r="47">
@@ -1309,7 +1309,7 @@
         <v>1290.0</v>
       </c>
       <c r="F47" t="n">
-        <v>0.11085271317829458</v>
+        <v>11.085271317829458</v>
       </c>
     </row>
     <row r="48">
@@ -1329,7 +1329,7 @@
         <v>1290.0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.13023255813953488</v>
+        <v>13.023255813953488</v>
       </c>
     </row>
     <row r="49">
@@ -1349,7 +1349,7 @@
         <v>1290.0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.1186046511627907</v>
+        <v>11.86046511627907</v>
       </c>
     </row>
     <row r="50">
@@ -1369,7 +1369,7 @@
         <v>1290.0</v>
       </c>
       <c r="F50" t="n">
-        <v>0.12015503875968993</v>
+        <v>12.015503875968992</v>
       </c>
     </row>
     <row r="51">
@@ -1389,7 +1389,7 @@
         <v>1290.0</v>
       </c>
       <c r="F51" t="n">
-        <v>0.09612403100775194</v>
+        <v>9.612403100775193</v>
       </c>
     </row>
     <row r="52">
@@ -1409,7 +1409,7 @@
         <v>1290.0</v>
       </c>
       <c r="F52" t="n">
-        <v>0.07286821705426356</v>
+        <v>7.286821705426356</v>
       </c>
     </row>
     <row r="53">
@@ -1429,7 +1429,7 @@
         <v>1290.0</v>
       </c>
       <c r="F53" t="n">
-        <v>0.07209302325581396</v>
+        <v>7.209302325581396</v>
       </c>
     </row>
     <row r="54">
@@ -1449,7 +1449,7 @@
         <v>1290.0</v>
       </c>
       <c r="F54" t="n">
-        <v>0.06046511627906977</v>
+        <v>6.046511627906977</v>
       </c>
     </row>
     <row r="55">
@@ -1469,7 +1469,7 @@
         <v>1290.0</v>
       </c>
       <c r="F55" t="n">
-        <v>0.02945736434108527</v>
+        <v>2.945736434108527</v>
       </c>
     </row>
     <row r="56">
@@ -1489,7 +1489,7 @@
         <v>1290.0</v>
       </c>
       <c r="F56" t="n">
-        <v>0.14806201550387596</v>
+        <v>14.806201550387597</v>
       </c>
     </row>
     <row r="57">
@@ -1509,7 +1509,7 @@
         <v>726.0</v>
       </c>
       <c r="F57" t="n">
-        <v>0.028925619834710745</v>
+        <v>2.8925619834710745</v>
       </c>
     </row>
     <row r="58">
@@ -1529,7 +1529,7 @@
         <v>726.0</v>
       </c>
       <c r="F58" t="n">
-        <v>0.07713498622589532</v>
+        <v>7.7134986225895315</v>
       </c>
     </row>
     <row r="59">
@@ -1549,7 +1549,7 @@
         <v>726.0</v>
       </c>
       <c r="F59" t="n">
-        <v>0.11019283746556474</v>
+        <v>11.019283746556475</v>
       </c>
     </row>
     <row r="60">
@@ -1569,7 +1569,7 @@
         <v>726.0</v>
       </c>
       <c r="F60" t="n">
-        <v>0.10192837465564739</v>
+        <v>10.192837465564738</v>
       </c>
     </row>
     <row r="61">
@@ -1589,7 +1589,7 @@
         <v>726.0</v>
       </c>
       <c r="F61" t="n">
-        <v>0.1046831955922865</v>
+        <v>10.46831955922865</v>
       </c>
     </row>
     <row r="62">
@@ -1609,7 +1609,7 @@
         <v>726.0</v>
       </c>
       <c r="F62" t="n">
-        <v>0.10192837465564739</v>
+        <v>10.192837465564738</v>
       </c>
     </row>
     <row r="63">
@@ -1629,7 +1629,7 @@
         <v>726.0</v>
       </c>
       <c r="F63" t="n">
-        <v>0.07024793388429752</v>
+        <v>7.024793388429752</v>
       </c>
     </row>
     <row r="64">
@@ -1649,7 +1649,7 @@
         <v>726.0</v>
       </c>
       <c r="F64" t="n">
-        <v>0.06336088154269973</v>
+        <v>6.336088154269973</v>
       </c>
     </row>
     <row r="65">
@@ -1669,7 +1669,7 @@
         <v>726.0</v>
       </c>
       <c r="F65" t="n">
-        <v>0.04132231404958678</v>
+        <v>4.132231404958678</v>
       </c>
     </row>
     <row r="66">
@@ -1689,7 +1689,7 @@
         <v>726.0</v>
       </c>
       <c r="F66" t="n">
-        <v>0.05234159779614325</v>
+        <v>5.234159779614325</v>
       </c>
     </row>
     <row r="67">
@@ -1709,7 +1709,7 @@
         <v>726.0</v>
       </c>
       <c r="F67" t="n">
-        <v>0.24793388429752067</v>
+        <v>24.793388429752067</v>
       </c>
     </row>
     <row r="68">
@@ -1729,7 +1729,7 @@
         <v>448.0</v>
       </c>
       <c r="F68" t="n">
-        <v>0.044642857142857144</v>
+        <v>4.464285714285714</v>
       </c>
     </row>
     <row r="69">
@@ -1749,7 +1749,7 @@
         <v>448.0</v>
       </c>
       <c r="F69" t="n">
-        <v>0.078125</v>
+        <v>7.8125</v>
       </c>
     </row>
     <row r="70">
@@ -1769,7 +1769,7 @@
         <v>448.0</v>
       </c>
       <c r="F70" t="n">
-        <v>0.09598214285714286</v>
+        <v>9.598214285714286</v>
       </c>
     </row>
     <row r="71">
@@ -1789,7 +1789,7 @@
         <v>448.0</v>
       </c>
       <c r="F71" t="n">
-        <v>0.09151785714285714</v>
+        <v>9.151785714285714</v>
       </c>
     </row>
     <row r="72">
@@ -1809,7 +1809,7 @@
         <v>448.0</v>
       </c>
       <c r="F72" t="n">
-        <v>0.08482142857142858</v>
+        <v>8.482142857142858</v>
       </c>
     </row>
     <row r="73">
@@ -1829,7 +1829,7 @@
         <v>448.0</v>
       </c>
       <c r="F73" t="n">
-        <v>0.078125</v>
+        <v>7.8125</v>
       </c>
     </row>
     <row r="74">
@@ -1849,7 +1849,7 @@
         <v>448.0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.09151785714285714</v>
+        <v>9.151785714285714</v>
       </c>
     </row>
     <row r="75">
@@ -1869,7 +1869,7 @@
         <v>448.0</v>
       </c>
       <c r="F75" t="n">
-        <v>0.049107142857142856</v>
+        <v>4.910714285714286</v>
       </c>
     </row>
     <row r="76">
@@ -1889,7 +1889,7 @@
         <v>448.0</v>
       </c>
       <c r="F76" t="n">
-        <v>0.049107142857142856</v>
+        <v>4.910714285714286</v>
       </c>
     </row>
     <row r="77">
@@ -1909,7 +1909,7 @@
         <v>448.0</v>
       </c>
       <c r="F77" t="n">
-        <v>0.04241071428571429</v>
+        <v>4.241071428571429</v>
       </c>
     </row>
     <row r="78">
@@ -1929,7 +1929,7 @@
         <v>448.0</v>
       </c>
       <c r="F78" t="n">
-        <v>0.29464285714285715</v>
+        <v>29.464285714285715</v>
       </c>
     </row>
     <row r="79">
@@ -1949,7 +1949,7 @@
         <v>54.0</v>
       </c>
       <c r="F79" t="n">
-        <v>0.018518518518518517</v>
+        <v>1.8518518518518516</v>
       </c>
     </row>
     <row r="80">
@@ -1969,7 +1969,7 @@
         <v>54.0</v>
       </c>
       <c r="F80" t="n">
-        <v>0.07407407407407407</v>
+        <v>7.4074074074074066</v>
       </c>
     </row>
     <row r="81">
@@ -1989,7 +1989,7 @@
         <v>54.0</v>
       </c>
       <c r="F81" t="n">
-        <v>0.037037037037037035</v>
+        <v>3.7037037037037033</v>
       </c>
     </row>
     <row r="82">
@@ -2009,7 +2009,7 @@
         <v>54.0</v>
       </c>
       <c r="F82" t="n">
-        <v>0.07407407407407407</v>
+        <v>7.4074074074074066</v>
       </c>
     </row>
     <row r="83">
@@ -2029,7 +2029,7 @@
         <v>54.0</v>
       </c>
       <c r="F83" t="n">
-        <v>0.09259259259259259</v>
+        <v>9.25925925925926</v>
       </c>
     </row>
     <row r="84">
@@ -2049,7 +2049,7 @@
         <v>54.0</v>
       </c>
       <c r="F84" t="n">
-        <v>0.07407407407407407</v>
+        <v>7.4074074074074066</v>
       </c>
     </row>
     <row r="85">
@@ -2069,7 +2069,7 @@
         <v>54.0</v>
       </c>
       <c r="F85" t="n">
-        <v>0.037037037037037035</v>
+        <v>3.7037037037037033</v>
       </c>
     </row>
     <row r="86">
@@ -2089,7 +2089,7 @@
         <v>54.0</v>
       </c>
       <c r="F86" t="n">
-        <v>0.037037037037037035</v>
+        <v>3.7037037037037033</v>
       </c>
     </row>
     <row r="87">
@@ -2109,7 +2109,7 @@
         <v>54.0</v>
       </c>
       <c r="F87" t="n">
-        <v>0.07407407407407407</v>
+        <v>7.4074074074074066</v>
       </c>
     </row>
     <row r="88">
@@ -2129,7 +2129,7 @@
         <v>54.0</v>
       </c>
       <c r="F88" t="n">
-        <v>0.05555555555555555</v>
+        <v>5.555555555555555</v>
       </c>
     </row>
     <row r="89">
@@ -2149,7 +2149,7 @@
         <v>54.0</v>
       </c>
       <c r="F89" t="n">
-        <v>0.42592592592592593</v>
+        <v>42.592592592592595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Graph x axis updates label
</commit_message>
<xml_diff>
--- a/data_output/eng_plot_input.xlsx
+++ b/data_output/eng_plot_input.xlsx
@@ -293,37 +293,37 @@
     <t>88</t>
   </si>
   <si>
-    <t>Less than 200</t>
-  </si>
-  <si>
-    <t>200 and less than  400</t>
-  </si>
-  <si>
-    <t>400 and less than 600</t>
-  </si>
-  <si>
-    <t>600 and less than 800</t>
-  </si>
-  <si>
-    <t>800 and less than 1000</t>
-  </si>
-  <si>
-    <t>1000 and less than 1200</t>
-  </si>
-  <si>
-    <t>1200 and less than 1400</t>
-  </si>
-  <si>
-    <t>1400 and less than 1600</t>
-  </si>
-  <si>
-    <t>1600 and less than 1800</t>
-  </si>
-  <si>
-    <t>1800 and less than 2000</t>
-  </si>
-  <si>
-    <t>Above 2000</t>
+    <t>Less than 10K</t>
+  </si>
+  <si>
+    <t>10K and less than  21K</t>
+  </si>
+  <si>
+    <t>20K and less than 31K</t>
+  </si>
+  <si>
+    <t>31K and less than 42K</t>
+  </si>
+  <si>
+    <t>42K and less than 52K</t>
+  </si>
+  <si>
+    <t>52K and less than 62K</t>
+  </si>
+  <si>
+    <t>62K and less than 73K</t>
+  </si>
+  <si>
+    <t>73K and less than 84K</t>
+  </si>
+  <si>
+    <t>84K and less than 94K</t>
+  </si>
+  <si>
+    <t>94K and less than 100K</t>
+  </si>
+  <si>
+    <t>Above 100K</t>
   </si>
 </sst>
 </file>

</xml_diff>